<commit_message>
Update day 24 for SEGCC account
</commit_message>
<xml_diff>
--- a/visualizations/day23.xlsx
+++ b/visualizations/day23.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danth\rust\aoc2021\visualizations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thordani\github_personal\aoc2021\visualizations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02304E47-B757-4C54-B754-C3A23F1ED901}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD457CCF-821D-4E37-967C-8F064DB86470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18015" windowHeight="13800" activeTab="1" xr2:uid="{18881BAB-96BC-4FC6-9585-DBAB2BA7479E}"/>
+    <workbookView xWindow="1905" yWindow="2550" windowWidth="21975" windowHeight="16215" activeTab="2" xr2:uid="{18881BAB-96BC-4FC6-9585-DBAB2BA7479E}"/>
   </bookViews>
   <sheets>
     <sheet name="Day23" sheetId="1" r:id="rId1"/>
     <sheet name="Day24" sheetId="2" r:id="rId2"/>
+    <sheet name="Day24_SEGCC" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="15">
   <si>
     <t>A</t>
   </si>
@@ -117,12 +118,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="9">
@@ -240,9 +247,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -259,11 +263,20 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -573,6 +586,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{402EAF34-7F52-4748-8815-64ED8E555BD3}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -621,11 +635,11 @@
       <c r="A4" s="7">
         <v>4</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1">
         <v>5</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="8">
         <v>7</v>
       </c>
     </row>
@@ -633,35 +647,35 @@
       <c r="A5" s="7">
         <v>5</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="1">
         <v>2</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="9"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="8"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="7"/>
-      <c r="B6" s="8">
+      <c r="B6" s="1">
         <v>7</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="9"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="8"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="7"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1">
         <v>7</v>
       </c>
-      <c r="D7" s="9"/>
+      <c r="D7" s="8"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
+      <c r="A8" s="9">
         <v>9</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="12"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="11"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -703,7 +717,7 @@
         <f>SUM(A10:D10)</f>
         <v>10608</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="F10" s="12" t="s">
         <v>9</v>
       </c>
     </row>
@@ -747,8 +761,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="14" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A20" s="14" t="s">
+    <row r="20" spans="1:4" s="13" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A20" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -780,35 +794,35 @@
       <c r="A23" s="7">
         <v>8</v>
       </c>
-      <c r="B23" s="8">
+      <c r="B23" s="1">
         <v>3</v>
       </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="9"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="8"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>5</v>
       </c>
-      <c r="B24" s="8">
+      <c r="B24" s="1">
         <v>4</v>
       </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="9"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="8"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8">
+      <c r="B25" s="1"/>
+      <c r="C25" s="1">
         <v>18</v>
       </c>
-      <c r="D25" s="9"/>
+      <c r="D25" s="8"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
-      <c r="B26" s="8"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="9">
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="8">
         <v>10</v>
       </c>
     </row>
@@ -816,69 +830,69 @@
       <c r="A27" s="7">
         <v>5</v>
       </c>
-      <c r="B27" s="8">
+      <c r="B27" s="1">
         <v>6</v>
       </c>
-      <c r="C27" s="8"/>
-      <c r="D27" s="9"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="8"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
-      <c r="B28" s="8">
+      <c r="B28" s="1">
         <v>4</v>
       </c>
-      <c r="C28" s="8">
+      <c r="C28" s="1">
         <v>6</v>
       </c>
-      <c r="D28" s="9"/>
+      <c r="D28" s="8"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>5</v>
       </c>
-      <c r="B29" s="8">
+      <c r="B29" s="1">
         <v>4</v>
       </c>
-      <c r="C29" s="8"/>
-      <c r="D29" s="9"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="8"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
-      <c r="B30" s="8">
+      <c r="B30" s="1">
         <v>11</v>
       </c>
-      <c r="C30" s="8"/>
-      <c r="D30" s="9"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="8"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
         <v>2</v>
       </c>
-      <c r="B31" s="8">
+      <c r="B31" s="1">
         <v>11</v>
       </c>
-      <c r="C31" s="8"/>
-      <c r="D31" s="9"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="8"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
         <v>6</v>
       </c>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8">
+      <c r="B32" s="1"/>
+      <c r="C32" s="1">
         <v>9</v>
       </c>
-      <c r="D32" s="9">
+      <c r="D32" s="8">
         <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="10">
+      <c r="A33" s="9">
         <v>28</v>
       </c>
-      <c r="B33" s="11"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="12"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="11"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
@@ -920,7 +934,7 @@
         <f>SUM(A35:D35)</f>
         <v>40799</v>
       </c>
-      <c r="F35" s="13" t="s">
+      <c r="F35" s="12" t="s">
         <v>9</v>
       </c>
     </row>
@@ -964,10 +978,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A26063A-D7E8-4B9E-AD26-DEE6AF567A1D}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1308,4 +1323,358 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4FF2A32-CE7D-42CB-9A43-7450C2D70CFC}">
+  <sheetPr codeName="Sheet3"/>
+  <dimension ref="A1:G15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>14</v>
+      </c>
+      <c r="C2">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <f>D2+C2</f>
+        <v>15</v>
+      </c>
+      <c r="G2">
+        <f>E2+F2</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <f>D3+C3+G2*26</f>
+        <v>400</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G15" si="0">E3+F3</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E10" si="1">D4+C4+G3*26</f>
+        <v>10405</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>10405</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>14</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>270544</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>270544</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ref="E6" si="2">D6+C6+G5*26</f>
+        <v>7034152</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>7034152</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>-7</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7" s="14">
+        <f t="shared" ref="D7:D15" si="3">MOD(G6,26)+B7</f>
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <f>INT(G6/26)</f>
+        <v>270544</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="0"/>
+        <v>270544</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>-13</v>
+      </c>
+      <c r="C8">
+        <v>15</v>
+      </c>
+      <c r="D8" s="14">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <f>INT(G7/26)</f>
+        <v>10405</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="0"/>
+        <v>10405</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>14</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ref="E9" si="4">D9+C9+G8*26</f>
+        <v>270545</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="0"/>
+        <v>270545</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>-7</v>
+      </c>
+      <c r="C10">
+        <v>6</v>
+      </c>
+      <c r="D10" s="14">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="F10">
+        <f>INT(G9/26)</f>
+        <v>10405</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="0"/>
+        <v>10405</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>11</v>
+      </c>
+      <c r="C11">
+        <v>14</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <f t="shared" ref="E10:E11" si="5">D11+C11+G10*26</f>
+        <v>270545</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="0"/>
+        <v>270545</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>-9</v>
+      </c>
+      <c r="C12">
+        <v>8</v>
+      </c>
+      <c r="D12" s="14">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="F12">
+        <f t="shared" ref="F11:F15" si="6">INT(G11/26)</f>
+        <v>10405</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>10405</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>-2</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="D13" s="14">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="6"/>
+        <v>400</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="0"/>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>-9</v>
+      </c>
+      <c r="C14">
+        <v>14</v>
+      </c>
+      <c r="D14" s="14">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>-14</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15" s="14">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D2:D15">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>A2&lt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>